<commit_message>
Refined PIR handling and script
</commit_message>
<xml_diff>
--- a/src/config/ElectricalSpec.xlsx
+++ b/src/config/ElectricalSpec.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/31ea737912db474e/Building/Fallow Barn/Lighting/Electrical/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="683" documentId="8_{EF94AAC1-67E7-47CF-9905-7FB49E5A84B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F690C7AD-325F-463E-BAF8-37371B2EC93D}"/>
+  <xr:revisionPtr revIDLastSave="707" documentId="8_{EF94AAC1-67E7-47CF-9905-7FB49E5A84B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46A46C6C-9306-45E8-A00F-99D8551F5622}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" tabRatio="500" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2389" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2416" uniqueCount="599">
   <si>
     <t>Wattage / unit</t>
   </si>
@@ -3047,13 +3047,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1101"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1102">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -4300,10 +4301,10 @@
     <tableColumn id="1" xr3:uid="{D85C7244-9E79-43DE-B77A-7B8DF63DE991}" name="Device"/>
     <tableColumn id="2" xr3:uid="{5534E196-4E76-4420-82D1-3025359EC286}" name="Start"/>
     <tableColumn id="3" xr3:uid="{33E1A706-C08C-4B49-9AB8-3EDB66702A7F}" name="Length"/>
-    <tableColumn id="4" xr3:uid="{121016CB-7F17-40A7-9EF0-85C16044DABC}" name="From" dataDxfId="4">
+    <tableColumn id="4" xr3:uid="{121016CB-7F17-40A7-9EF0-85C16044DABC}" name="From" dataDxfId="2">
       <calculatedColumnFormula>subnetStart&amp;IPConfig[[#This Row],[Start]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{0E14B759-2635-4066-A904-6861AEB274CE}" name="To" dataDxfId="3">
+    <tableColumn id="5" xr3:uid="{0E14B759-2635-4066-A904-6861AEB274CE}" name="To" dataDxfId="1">
       <calculatedColumnFormula>subnetStart&amp;(IPConfig[[#This Row],[Start]]+IPConfig[[#This Row],[Length]]-1)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4334,7 +4335,7 @@
     <tableColumn id="8" xr3:uid="{267B77D7-F518-4304-9194-660D0C25C51C}" name="brightness"/>
     <tableColumn id="9" xr3:uid="{6F3B9475-A57D-4286-918F-D9433DB65CF8}" name="transition_duration"/>
     <tableColumn id="10" xr3:uid="{DEEC1C2A-8664-40E8-B521-4D52622F778A}" name="toggle_after"/>
-    <tableColumn id="11" xr3:uid="{74E94DD4-F16D-4226-A7C1-6E75688D44DB}" name="url" dataDxfId="2">
+    <tableColumn id="11" xr3:uid="{74E94DD4-F16D-4226-A7C1-6E75688D44DB}" name="url" dataDxfId="0">
       <calculatedColumnFormula>"http://[ip]/rpc/"&amp;StateSets[[#This Row],[type]]&amp;".Set?id="&amp;StateSets[[#This Row],[id]]&amp;"&amp;on="&amp;StateSets[[#This Row],[on]]&amp; IF(StateSets[[#This Row],[brightness]]&gt;0, "&amp;brightness="&amp;StateSets[[#This Row],[brightness]], "") &amp; IF(StateSets[[#This Row],[transition_duration]]&gt;0, "&amp;transition_duration=" &amp; StateSets[[#This Row],[transition_duration]], "") &amp; IF(StateSets[[#This Row],[toggle_after]]&gt;0, "&amp;toggle_after=" &amp; StateSets[[#This Row],[toggle_after]], "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4536,17 +4537,17 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BEA59DA5-7029-42D4-A08E-2FE79AB0AA0D}" name="Table2" displayName="Table2" ref="A1:K55" totalsRowShown="0">
-  <autoFilter ref="A1:K55" xr:uid="{BEA59DA5-7029-42D4-A08E-2FE79AB0AA0D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BEA59DA5-7029-42D4-A08E-2FE79AB0AA0D}" name="Table2" displayName="Table2" ref="A1:K60" totalsRowShown="0">
+  <autoFilter ref="A1:K60" xr:uid="{BEA59DA5-7029-42D4-A08E-2FE79AB0AA0D}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{9AD75D2B-6EB2-4FE9-ABEC-A3D47AA92C0D}" name="lookup Room"/>
     <tableColumn id="2" xr3:uid="{56AC9673-AD2C-4058-B28A-145F2F3F1213}" name="lookup Device"/>
-    <tableColumn id="7" xr3:uid="{E393F2DF-77CC-4350-BB8F-BC1F15B155FC}" name="start" dataDxfId="1">
+    <tableColumn id="7" xr3:uid="{E393F2DF-77CC-4350-BB8F-BC1F15B155FC}" name="start" dataDxfId="7">
       <calculatedColumnFormula array="1">_xlfn.XLOOKUP(1,(LightSpec[Location]=Table2[[#This Row],[lookup Room]]) * (LightSpec[DiagNo]=Table2[[#This Row],[lookup Device]]), LightSpec[startinput])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{AF27997C-363A-48C4-B07C-36FBB8253D24}" name="Trigger"/>
     <tableColumn id="4" xr3:uid="{CEF6CA50-B7D9-4D2D-83E3-9743E522D4D3}" name="trigger_event"/>
-    <tableColumn id="5" xr3:uid="{FB455A92-6BFA-4CD1-A617-15992E655AB9}" name="trigger_device" dataDxfId="7">
+    <tableColumn id="5" xr3:uid="{FB455A92-6BFA-4CD1-A617-15992E655AB9}" name="trigger_device" dataDxfId="6">
       <calculatedColumnFormula array="1">_xlfn.LET(
   _xlpm.txt, _xlfn.XLOOKUP(1,(LightSpec[Location]=Table2[[#This Row],[lookup Room]]) * (LightSpec[DiagNo]=Table2[[#This Row],[lookup Device]]),LightSpec[From]),
   _xlpm.n, LEN(_xlpm.txt),
@@ -4554,14 +4555,14 @@
   LEFT(_xlpm.txt, _xlpm.pos)
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{4BD12DA4-A050-40B5-9C17-B8F069EE8B05}" name="input" dataDxfId="0">
+    <tableColumn id="6" xr3:uid="{4BD12DA4-A050-40B5-9C17-B8F069EE8B05}" name="input" dataDxfId="5">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Table2[[#This Row],[Trigger]],SwitchButtons[switch],SwitchButtons[input])+Table2[[#This Row],[start]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{F26FF3DE-D392-4E9F-83C6-43F73BD62F47}" name="set1"/>
-    <tableColumn id="10" xr3:uid="{20EF778F-ECB3-4159-808E-4C276D480DE4}" name="set1_device" dataDxfId="6">
+    <tableColumn id="10" xr3:uid="{20EF778F-ECB3-4159-808E-4C276D480DE4}" name="set1_device" dataDxfId="4">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Table2[[#This Row],[set1]],circuitoutputs[circuit],circuitoutputs[device])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{D92B0F03-8683-4FD4-BBC9-0B036EFFC133}" name="set1_output" dataDxfId="5">
+    <tableColumn id="11" xr3:uid="{D92B0F03-8683-4FD4-BBC9-0B036EFFC133}" name="set1_output" dataDxfId="3">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Table2[[#This Row],[set1]],circuitoutputs[circuit],circuitoutputs[output])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="12" xr3:uid="{0E6D6891-1F2E-4355-8CC3-008DCBD11CA5}" name="set1_brightness"/>
@@ -5100,7 +5101,7 @@
   <dimension ref="A1:W214"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -27244,10 +27245,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0BC4206-4141-4753-AE9C-AE20F6BE091A}">
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="K60" sqref="K60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -29107,17 +29108,17 @@
       <c r="B42" t="s">
         <v>196</v>
       </c>
-      <c r="C42" cm="1">
+      <c r="C42" s="6" cm="1">
         <f t="array" ref="C42">_xlfn.XLOOKUP(1,(LightSpec[Location]=Table2[[#This Row],[lookup Room]]) * (LightSpec[DiagNo]=Table2[[#This Row],[lookup Device]]), LightSpec[startinput])</f>
         <v>0</v>
       </c>
       <c r="D42" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E42" t="s">
-        <v>505</v>
-      </c>
-      <c r="F42" t="str" cm="1">
+        <v>508</v>
+      </c>
+      <c r="F42" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="F42" ca="1">_xlfn.LET(
   _xlpm.txt, _xlfn.XLOOKUP(1,(LightSpec[Location]=Table2[[#This Row],[lookup Room]]) * (LightSpec[DiagNo]=Table2[[#This Row],[lookup Device]]),LightSpec[From]),
   _xlpm.n, LEN(_xlpm.txt),
@@ -29126,23 +29127,23 @@
 )</f>
         <v>D3</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="6">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Trigger]],SwitchButtons[switch],SwitchButtons[input])+Table2[[#This Row],[start]]</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H42" t="s">
         <v>522</v>
       </c>
-      <c r="I42" t="str">
+      <c r="I42" s="6" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[set1]],circuitoutputs[circuit],circuitoutputs[device])</f>
         <v>D2</v>
       </c>
-      <c r="J42">
+      <c r="J42" s="6">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[set1]],circuitoutputs[circuit],circuitoutputs[output])</f>
         <v>0</v>
       </c>
-      <c r="K42" t="s">
-        <v>500</v>
+      <c r="K42">
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.6">
@@ -29152,17 +29153,17 @@
       <c r="B43" t="s">
         <v>196</v>
       </c>
-      <c r="C43" cm="1">
+      <c r="C43" s="6" cm="1">
         <f t="array" ref="C43">_xlfn.XLOOKUP(1,(LightSpec[Location]=Table2[[#This Row],[lookup Room]]) * (LightSpec[DiagNo]=Table2[[#This Row],[lookup Device]]), LightSpec[startinput])</f>
         <v>0</v>
       </c>
       <c r="D43" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E43" t="s">
-        <v>505</v>
-      </c>
-      <c r="F43" t="str" cm="1">
+        <v>508</v>
+      </c>
+      <c r="F43" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="F43" ca="1">_xlfn.LET(
   _xlpm.txt, _xlfn.XLOOKUP(1,(LightSpec[Location]=Table2[[#This Row],[lookup Room]]) * (LightSpec[DiagNo]=Table2[[#This Row],[lookup Device]]),LightSpec[From]),
   _xlpm.n, LEN(_xlpm.txt),
@@ -29171,23 +29172,23 @@
 )</f>
         <v>D3</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="6">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Trigger]],SwitchButtons[switch],SwitchButtons[input])+Table2[[#This Row],[start]]</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H43" t="s">
         <v>523</v>
       </c>
-      <c r="I43" t="str">
+      <c r="I43" s="6" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[set1]],circuitoutputs[circuit],circuitoutputs[device])</f>
         <v>D3</v>
       </c>
-      <c r="J43">
+      <c r="J43" s="6">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[set1]],circuitoutputs[circuit],circuitoutputs[output])</f>
         <v>0</v>
       </c>
-      <c r="K43" t="s">
-        <v>500</v>
+      <c r="K43">
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.6">
@@ -29197,17 +29198,17 @@
       <c r="B44" t="s">
         <v>196</v>
       </c>
-      <c r="C44" cm="1">
+      <c r="C44" s="6" cm="1">
         <f t="array" ref="C44">_xlfn.XLOOKUP(1,(LightSpec[Location]=Table2[[#This Row],[lookup Room]]) * (LightSpec[DiagNo]=Table2[[#This Row],[lookup Device]]), LightSpec[startinput])</f>
         <v>0</v>
       </c>
       <c r="D44" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E44" t="s">
-        <v>505</v>
-      </c>
-      <c r="F44" t="str" cm="1">
+        <v>508</v>
+      </c>
+      <c r="F44" s="6" t="str" cm="1">
         <f t="array" aca="1" ref="F44" ca="1">_xlfn.LET(
   _xlpm.txt, _xlfn.XLOOKUP(1,(LightSpec[Location]=Table2[[#This Row],[lookup Room]]) * (LightSpec[DiagNo]=Table2[[#This Row],[lookup Device]]),LightSpec[From]),
   _xlpm.n, LEN(_xlpm.txt),
@@ -29216,23 +29217,23 @@
 )</f>
         <v>D3</v>
       </c>
-      <c r="G44">
+      <c r="G44" s="6">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Trigger]],SwitchButtons[switch],SwitchButtons[input])+Table2[[#This Row],[start]]</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H44" t="s">
         <v>560</v>
       </c>
-      <c r="I44" t="str">
+      <c r="I44" s="6" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[set1]],circuitoutputs[circuit],circuitoutputs[device])</f>
         <v>D3</v>
       </c>
-      <c r="J44">
+      <c r="J44" s="6">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[set1]],circuitoutputs[circuit],circuitoutputs[output])</f>
         <v>1</v>
       </c>
-      <c r="K44" t="s">
-        <v>500</v>
+      <c r="K44">
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.6">
@@ -29247,7 +29248,7 @@
         <v>0</v>
       </c>
       <c r="D45" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E45" t="s">
         <v>505</v>
@@ -29263,21 +29264,21 @@
       </c>
       <c r="G45">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Trigger]],SwitchButtons[switch],SwitchButtons[input])+Table2[[#This Row],[start]]</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H45" t="s">
-        <v>535</v>
+        <v>522</v>
       </c>
       <c r="I45" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[set1]],circuitoutputs[circuit],circuitoutputs[device])</f>
-        <v>D15</v>
+        <v>D2</v>
       </c>
       <c r="J45">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[set1]],circuitoutputs[circuit],circuitoutputs[output])</f>
         <v>0</v>
       </c>
       <c r="K45" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.6">
@@ -29292,7 +29293,7 @@
         <v>0</v>
       </c>
       <c r="D46" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E46" t="s">
         <v>505</v>
@@ -29308,21 +29309,21 @@
       </c>
       <c r="G46">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Trigger]],SwitchButtons[switch],SwitchButtons[input])+Table2[[#This Row],[start]]</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H46" t="s">
-        <v>570</v>
+        <v>523</v>
       </c>
       <c r="I46" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[set1]],circuitoutputs[circuit],circuitoutputs[device])</f>
-        <v>D15</v>
+        <v>D3</v>
       </c>
       <c r="J46">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[set1]],circuitoutputs[circuit],circuitoutputs[output])</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K46" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.6">
@@ -29337,7 +29338,7 @@
         <v>0</v>
       </c>
       <c r="D47" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E47" t="s">
         <v>505</v>
@@ -29353,21 +29354,21 @@
       </c>
       <c r="G47">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Trigger]],SwitchButtons[switch],SwitchButtons[input])+Table2[[#This Row],[start]]</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H47" t="s">
-        <v>536</v>
+        <v>560</v>
       </c>
       <c r="I47" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[set1]],circuitoutputs[circuit],circuitoutputs[device])</f>
-        <v>D16</v>
+        <v>D3</v>
       </c>
       <c r="J47">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[set1]],circuitoutputs[circuit],circuitoutputs[output])</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K47" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.6">
@@ -29385,7 +29386,7 @@
         <v>449</v>
       </c>
       <c r="E48" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="F48" t="str" cm="1">
         <f t="array" aca="1" ref="F48" ca="1">_xlfn.LET(
@@ -29411,8 +29412,8 @@
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[set1]],circuitoutputs[circuit],circuitoutputs[output])</f>
         <v>0</v>
       </c>
-      <c r="K48">
-        <v>100</v>
+      <c r="K48" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.6">
@@ -29430,7 +29431,7 @@
         <v>449</v>
       </c>
       <c r="E49" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="F49" t="str" cm="1">
         <f t="array" aca="1" ref="F49" ca="1">_xlfn.LET(
@@ -29456,8 +29457,8 @@
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[set1]],circuitoutputs[circuit],circuitoutputs[output])</f>
         <v>1</v>
       </c>
-      <c r="K49">
-        <v>100</v>
+      <c r="K49" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.6">
@@ -29475,7 +29476,7 @@
         <v>449</v>
       </c>
       <c r="E50" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="F50" t="str" cm="1">
         <f t="array" aca="1" ref="F50" ca="1">_xlfn.LET(
@@ -29501,8 +29502,8 @@
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[set1]],circuitoutputs[circuit],circuitoutputs[output])</f>
         <v>0</v>
       </c>
-      <c r="K50">
-        <v>100</v>
+      <c r="K50" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.6">
@@ -29517,10 +29518,10 @@
         <v>0</v>
       </c>
       <c r="D51" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E51" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="F51" t="str" cm="1">
         <f t="array" aca="1" ref="F51" ca="1">_xlfn.LET(
@@ -29533,7 +29534,7 @@
       </c>
       <c r="G51">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Trigger]],SwitchButtons[switch],SwitchButtons[input])+Table2[[#This Row],[start]]</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H51" t="s">
         <v>535</v>
@@ -29546,8 +29547,8 @@
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[set1]],circuitoutputs[circuit],circuitoutputs[output])</f>
         <v>0</v>
       </c>
-      <c r="K51" t="s">
-        <v>500</v>
+      <c r="K51">
+        <v>100</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.6">
@@ -29562,10 +29563,10 @@
         <v>0</v>
       </c>
       <c r="D52" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E52" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="F52" t="str" cm="1">
         <f t="array" aca="1" ref="F52" ca="1">_xlfn.LET(
@@ -29578,7 +29579,7 @@
       </c>
       <c r="G52">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Trigger]],SwitchButtons[switch],SwitchButtons[input])+Table2[[#This Row],[start]]</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H52" t="s">
         <v>570</v>
@@ -29591,8 +29592,8 @@
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[set1]],circuitoutputs[circuit],circuitoutputs[output])</f>
         <v>1</v>
       </c>
-      <c r="K52" t="s">
-        <v>500</v>
+      <c r="K52">
+        <v>100</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.6">
@@ -29607,10 +29608,10 @@
         <v>0</v>
       </c>
       <c r="D53" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E53" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="F53" t="str" cm="1">
         <f t="array" aca="1" ref="F53" ca="1">_xlfn.LET(
@@ -29623,7 +29624,7 @@
       </c>
       <c r="G53">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Trigger]],SwitchButtons[switch],SwitchButtons[input])+Table2[[#This Row],[start]]</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H53" t="s">
         <v>536</v>
@@ -29636,8 +29637,8 @@
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[set1]],circuitoutputs[circuit],circuitoutputs[output])</f>
         <v>0</v>
       </c>
-      <c r="K53" t="s">
-        <v>500</v>
+      <c r="K53">
+        <v>100</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.6">
@@ -29645,17 +29646,17 @@
         <v>181</v>
       </c>
       <c r="B54" t="s">
-        <v>253</v>
+        <v>196</v>
       </c>
       <c r="C54" cm="1">
         <f t="array" ref="C54">_xlfn.XLOOKUP(1,(LightSpec[Location]=Table2[[#This Row],[lookup Room]]) * (LightSpec[DiagNo]=Table2[[#This Row],[lookup Device]]), LightSpec[startinput])</f>
         <v>0</v>
       </c>
       <c r="D54" t="s">
-        <v>510</v>
+        <v>450</v>
       </c>
       <c r="E54" t="s">
-        <v>593</v>
+        <v>505</v>
       </c>
       <c r="F54" t="str" cm="1">
         <f t="array" aca="1" ref="F54" ca="1">_xlfn.LET(
@@ -29664,25 +29665,25 @@
   _xlpm.pos, MATCH(FALSE, ISNUMBER(MID(_xlpm.txt, ROW(INDIRECT("2:" &amp; _xlpm.n)), 1)*1), 0),
   LEFT(_xlpm.txt, _xlpm.pos)
 )</f>
-        <v>P1</v>
+        <v>D3</v>
       </c>
       <c r="G54">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Trigger]],SwitchButtons[switch],SwitchButtons[input])+Table2[[#This Row],[start]]</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H54" t="s">
-        <v>522</v>
+        <v>535</v>
       </c>
       <c r="I54" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[set1]],circuitoutputs[circuit],circuitoutputs[device])</f>
-        <v>D2</v>
+        <v>D15</v>
       </c>
       <c r="J54">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[set1]],circuitoutputs[circuit],circuitoutputs[output])</f>
         <v>0</v>
       </c>
       <c r="K54" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.6">
@@ -29690,17 +29691,17 @@
         <v>181</v>
       </c>
       <c r="B55" t="s">
-        <v>253</v>
+        <v>196</v>
       </c>
       <c r="C55" cm="1">
         <f t="array" ref="C55">_xlfn.XLOOKUP(1,(LightSpec[Location]=Table2[[#This Row],[lookup Room]]) * (LightSpec[DiagNo]=Table2[[#This Row],[lookup Device]]), LightSpec[startinput])</f>
         <v>0</v>
       </c>
       <c r="D55" t="s">
-        <v>510</v>
+        <v>450</v>
       </c>
       <c r="E55" t="s">
-        <v>594</v>
+        <v>505</v>
       </c>
       <c r="F55" t="str" cm="1">
         <f t="array" aca="1" ref="F55" ca="1">_xlfn.LET(
@@ -29709,39 +29710,264 @@
   _xlpm.pos, MATCH(FALSE, ISNUMBER(MID(_xlpm.txt, ROW(INDIRECT("2:" &amp; _xlpm.n)), 1)*1), 0),
   LEFT(_xlpm.txt, _xlpm.pos)
 )</f>
-        <v>P1</v>
+        <v>D3</v>
       </c>
       <c r="G55">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Trigger]],SwitchButtons[switch],SwitchButtons[input])+Table2[[#This Row],[start]]</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H55" t="s">
-        <v>522</v>
+        <v>570</v>
       </c>
       <c r="I55" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[set1]],circuitoutputs[circuit],circuitoutputs[device])</f>
-        <v>D2</v>
+        <v>D15</v>
       </c>
       <c r="J55">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[set1]],circuitoutputs[circuit],circuitoutputs[output])</f>
+        <v>1</v>
+      </c>
+      <c r="K55" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A56" t="s">
+        <v>181</v>
+      </c>
+      <c r="B56" t="s">
+        <v>196</v>
+      </c>
+      <c r="C56" cm="1">
+        <f t="array" ref="C56">_xlfn.XLOOKUP(1,(LightSpec[Location]=Table2[[#This Row],[lookup Room]]) * (LightSpec[DiagNo]=Table2[[#This Row],[lookup Device]]), LightSpec[startinput])</f>
         <v>0</v>
       </c>
-      <c r="K55" t="s">
+      <c r="D56" t="s">
+        <v>450</v>
+      </c>
+      <c r="E56" t="s">
+        <v>505</v>
+      </c>
+      <c r="F56" t="str" cm="1">
+        <f t="array" aca="1" ref="F56" ca="1">_xlfn.LET(
+  _xlpm.txt, _xlfn.XLOOKUP(1,(LightSpec[Location]=Table2[[#This Row],[lookup Room]]) * (LightSpec[DiagNo]=Table2[[#This Row],[lookup Device]]),LightSpec[From]),
+  _xlpm.n, LEN(_xlpm.txt),
+  _xlpm.pos, MATCH(FALSE, ISNUMBER(MID(_xlpm.txt, ROW(INDIRECT("2:" &amp; _xlpm.n)), 1)*1), 0),
+  LEFT(_xlpm.txt, _xlpm.pos)
+)</f>
+        <v>D3</v>
+      </c>
+      <c r="G56">
+        <f>_xlfn.XLOOKUP(Table2[[#This Row],[Trigger]],SwitchButtons[switch],SwitchButtons[input])+Table2[[#This Row],[start]]</f>
+        <v>3</v>
+      </c>
+      <c r="H56" t="s">
+        <v>536</v>
+      </c>
+      <c r="I56" t="str">
+        <f>_xlfn.XLOOKUP(Table2[[#This Row],[set1]],circuitoutputs[circuit],circuitoutputs[device])</f>
+        <v>D16</v>
+      </c>
+      <c r="J56">
+        <f>_xlfn.XLOOKUP(Table2[[#This Row],[set1]],circuitoutputs[circuit],circuitoutputs[output])</f>
+        <v>0</v>
+      </c>
+      <c r="K56" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A57" t="s">
+        <v>181</v>
+      </c>
+      <c r="B57" t="s">
+        <v>253</v>
+      </c>
+      <c r="C57" cm="1">
+        <f t="array" ref="C57">_xlfn.XLOOKUP(1,(LightSpec[Location]=Table2[[#This Row],[lookup Room]]) * (LightSpec[DiagNo]=Table2[[#This Row],[lookup Device]]), LightSpec[startinput])</f>
+        <v>0</v>
+      </c>
+      <c r="D57" t="s">
+        <v>510</v>
+      </c>
+      <c r="E57" t="s">
+        <v>593</v>
+      </c>
+      <c r="F57" t="str" cm="1">
+        <f t="array" aca="1" ref="F57" ca="1">_xlfn.LET(
+  _xlpm.txt, _xlfn.XLOOKUP(1,(LightSpec[Location]=Table2[[#This Row],[lookup Room]]) * (LightSpec[DiagNo]=Table2[[#This Row],[lookup Device]]),LightSpec[From]),
+  _xlpm.n, LEN(_xlpm.txt),
+  _xlpm.pos, MATCH(FALSE, ISNUMBER(MID(_xlpm.txt, ROW(INDIRECT("2:" &amp; _xlpm.n)), 1)*1), 0),
+  LEFT(_xlpm.txt, _xlpm.pos)
+)</f>
+        <v>P1</v>
+      </c>
+      <c r="G57">
+        <f>_xlfn.XLOOKUP(Table2[[#This Row],[Trigger]],SwitchButtons[switch],SwitchButtons[input])+Table2[[#This Row],[start]]</f>
+        <v>0</v>
+      </c>
+      <c r="H57" t="s">
+        <v>522</v>
+      </c>
+      <c r="I57" t="str">
+        <f>_xlfn.XLOOKUP(Table2[[#This Row],[set1]],circuitoutputs[circuit],circuitoutputs[device])</f>
+        <v>D2</v>
+      </c>
+      <c r="J57">
+        <f>_xlfn.XLOOKUP(Table2[[#This Row],[set1]],circuitoutputs[circuit],circuitoutputs[output])</f>
+        <v>0</v>
+      </c>
+      <c r="K57" t="s">
         <v>499</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A58" t="s">
+        <v>181</v>
+      </c>
+      <c r="B58" t="s">
+        <v>253</v>
+      </c>
+      <c r="C58" s="6" cm="1">
+        <f t="array" ref="C58">_xlfn.XLOOKUP(1,(LightSpec[Location]=Table2[[#This Row],[lookup Room]]) * (LightSpec[DiagNo]=Table2[[#This Row],[lookup Device]]), LightSpec[startinput])</f>
+        <v>0</v>
+      </c>
+      <c r="D58" t="s">
+        <v>510</v>
+      </c>
+      <c r="E58" t="s">
+        <v>593</v>
+      </c>
+      <c r="F58" s="6" t="str" cm="1">
+        <f t="array" aca="1" ref="F58" ca="1">_xlfn.LET(
+  _xlpm.txt, _xlfn.XLOOKUP(1,(LightSpec[Location]=Table2[[#This Row],[lookup Room]]) * (LightSpec[DiagNo]=Table2[[#This Row],[lookup Device]]),LightSpec[From]),
+  _xlpm.n, LEN(_xlpm.txt),
+  _xlpm.pos, MATCH(FALSE, ISNUMBER(MID(_xlpm.txt, ROW(INDIRECT("2:" &amp; _xlpm.n)), 1)*1), 0),
+  LEFT(_xlpm.txt, _xlpm.pos)
+)</f>
+        <v>P1</v>
+      </c>
+      <c r="G58" s="6">
+        <f>_xlfn.XLOOKUP(Table2[[#This Row],[Trigger]],SwitchButtons[switch],SwitchButtons[input])+Table2[[#This Row],[start]]</f>
+        <v>0</v>
+      </c>
+      <c r="H58" t="s">
+        <v>559</v>
+      </c>
+      <c r="I58" s="6" t="str">
+        <f>_xlfn.XLOOKUP(Table2[[#This Row],[set1]],circuitoutputs[circuit],circuitoutputs[device])</f>
+        <v>D2</v>
+      </c>
+      <c r="J58" s="6">
+        <f>_xlfn.XLOOKUP(Table2[[#This Row],[set1]],circuitoutputs[circuit],circuitoutputs[output])</f>
+        <v>1</v>
+      </c>
+      <c r="K58" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A59" t="s">
+        <v>181</v>
+      </c>
+      <c r="B59" t="s">
+        <v>253</v>
+      </c>
+      <c r="C59" cm="1">
+        <f t="array" ref="C59">_xlfn.XLOOKUP(1,(LightSpec[Location]=Table2[[#This Row],[lookup Room]]) * (LightSpec[DiagNo]=Table2[[#This Row],[lookup Device]]), LightSpec[startinput])</f>
+        <v>0</v>
+      </c>
+      <c r="D59" t="s">
+        <v>510</v>
+      </c>
+      <c r="E59" t="s">
+        <v>594</v>
+      </c>
+      <c r="F59" t="str" cm="1">
+        <f t="array" aca="1" ref="F59" ca="1">_xlfn.LET(
+  _xlpm.txt, _xlfn.XLOOKUP(1,(LightSpec[Location]=Table2[[#This Row],[lookup Room]]) * (LightSpec[DiagNo]=Table2[[#This Row],[lookup Device]]),LightSpec[From]),
+  _xlpm.n, LEN(_xlpm.txt),
+  _xlpm.pos, MATCH(FALSE, ISNUMBER(MID(_xlpm.txt, ROW(INDIRECT("2:" &amp; _xlpm.n)), 1)*1), 0),
+  LEFT(_xlpm.txt, _xlpm.pos)
+)</f>
+        <v>P1</v>
+      </c>
+      <c r="G59">
+        <f>_xlfn.XLOOKUP(Table2[[#This Row],[Trigger]],SwitchButtons[switch],SwitchButtons[input])+Table2[[#This Row],[start]]</f>
+        <v>0</v>
+      </c>
+      <c r="H59" t="s">
+        <v>522</v>
+      </c>
+      <c r="I59" t="str">
+        <f>_xlfn.XLOOKUP(Table2[[#This Row],[set1]],circuitoutputs[circuit],circuitoutputs[device])</f>
+        <v>D2</v>
+      </c>
+      <c r="J59">
+        <f>_xlfn.XLOOKUP(Table2[[#This Row],[set1]],circuitoutputs[circuit],circuitoutputs[output])</f>
+        <v>0</v>
+      </c>
+      <c r="K59" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.6">
+      <c r="A60" t="s">
+        <v>181</v>
+      </c>
+      <c r="B60" t="s">
+        <v>253</v>
+      </c>
+      <c r="C60" s="6" cm="1">
+        <f t="array" ref="C60">_xlfn.XLOOKUP(1,(LightSpec[Location]=Table2[[#This Row],[lookup Room]]) * (LightSpec[DiagNo]=Table2[[#This Row],[lookup Device]]), LightSpec[startinput])</f>
+        <v>0</v>
+      </c>
+      <c r="D60" t="s">
+        <v>510</v>
+      </c>
+      <c r="E60" t="s">
+        <v>594</v>
+      </c>
+      <c r="F60" s="6" t="str" cm="1">
+        <f t="array" aca="1" ref="F60" ca="1">_xlfn.LET(
+  _xlpm.txt, _xlfn.XLOOKUP(1,(LightSpec[Location]=Table2[[#This Row],[lookup Room]]) * (LightSpec[DiagNo]=Table2[[#This Row],[lookup Device]]),LightSpec[From]),
+  _xlpm.n, LEN(_xlpm.txt),
+  _xlpm.pos, MATCH(FALSE, ISNUMBER(MID(_xlpm.txt, ROW(INDIRECT("2:" &amp; _xlpm.n)), 1)*1), 0),
+  LEFT(_xlpm.txt, _xlpm.pos)
+)</f>
+        <v>P1</v>
+      </c>
+      <c r="G60" s="6">
+        <f>_xlfn.XLOOKUP(Table2[[#This Row],[Trigger]],SwitchButtons[switch],SwitchButtons[input])+Table2[[#This Row],[start]]</f>
+        <v>0</v>
+      </c>
+      <c r="H60" t="s">
+        <v>559</v>
+      </c>
+      <c r="I60" s="6" t="str">
+        <f>_xlfn.XLOOKUP(Table2[[#This Row],[set1]],circuitoutputs[circuit],circuitoutputs[device])</f>
+        <v>D2</v>
+      </c>
+      <c r="J60" s="6">
+        <f>_xlfn.XLOOKUP(Table2[[#This Row],[set1]],circuitoutputs[circuit],circuitoutputs[output])</f>
+        <v>1</v>
+      </c>
+      <c r="K60" t="s">
+        <v>500</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E55" xr:uid="{49429DE3-973E-403E-84EA-B8875915DFCC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E60" xr:uid="{49429DE3-973E-403E-84EA-B8875915DFCC}">
       <formula1>Events</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D55" xr:uid="{B2D9965E-1658-4CF4-B6FD-8B03F391884B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D60" xr:uid="{B2D9965E-1658-4CF4-B6FD-8B03F391884B}">
       <formula1>Trigger</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H55" xr:uid="{0807570B-CF24-4764-B4AE-B0A5505B97C5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H60" xr:uid="{0807570B-CF24-4764-B4AE-B0A5505B97C5}">
       <formula1>circuits</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K55" xr:uid="{201D99B1-86EC-4CF7-81FA-2F45C3C3A57E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K60" xr:uid="{201D99B1-86EC-4CF7-81FA-2F45C3C3A57E}">
       <formula1>Brightness</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>